<commit_message>
added space for more measurements
</commit_message>
<xml_diff>
--- a/assignment2_mb_results.xlsx
+++ b/assignment2_mb_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="6210" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="6210"/>
   </bookViews>
   <sheets>
     <sheet name="OpenMP" sheetId="1" r:id="rId1"/>
@@ -551,11 +551,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="40658048"/>
-        <c:axId val="40658624"/>
+        <c:axId val="109126208"/>
+        <c:axId val="109126784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="40658048"/>
+        <c:axId val="109126208"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -586,12 +586,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40658624"/>
+        <c:crossAx val="109126784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="40658624"/>
+        <c:axId val="109126784"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -626,7 +626,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40658048"/>
+        <c:crossAx val="109126208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -689,10 +689,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>OpenMP!$B$27:$F$27</c:f>
+              <c:f>OpenMP!$B$27:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -703,9 +703,12 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
@@ -713,10 +716,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>OpenMP!$B$28:$F$28</c:f>
+              <c:f>OpenMP!$B$28:$G$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>16.119</c:v>
                 </c:pt>
@@ -726,10 +729,10 @@
                 <c:pt idx="2">
                   <c:v>5.7969999999999997</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>5.5789999999999997</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>6.3559999999999999</c:v>
                 </c:pt>
               </c:numCache>
@@ -758,10 +761,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>OpenMP!$B$27:$F$27</c:f>
+              <c:f>OpenMP!$B$27:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -772,9 +775,12 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
@@ -782,10 +788,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>OpenMP!$B$29:$F$29</c:f>
+              <c:f>OpenMP!$B$29:$G$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>414.84199999999998</c:v>
                 </c:pt>
@@ -795,10 +801,10 @@
                 <c:pt idx="2">
                   <c:v>77.325000000000003</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>51.884999999999998</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>44.828000000000003</c:v>
                 </c:pt>
               </c:numCache>
@@ -827,10 +833,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>OpenMP!$B$27:$F$27</c:f>
+              <c:f>OpenMP!$B$27:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -841,9 +847,12 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
@@ -851,10 +860,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>OpenMP!$B$30:$F$30</c:f>
+              <c:f>OpenMP!$B$30:$G$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>2839.4</c:v>
                 </c:pt>
@@ -864,10 +873,10 @@
                 <c:pt idx="2">
                   <c:v>390.072</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>234.83599999999998</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>195.92000000000002</c:v>
                 </c:pt>
               </c:numCache>
@@ -883,11 +892,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="40660928"/>
-        <c:axId val="40661504"/>
+        <c:axId val="109129088"/>
+        <c:axId val="109129664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="40660928"/>
+        <c:axId val="109129088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -916,12 +925,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40661504"/>
+        <c:crossAx val="109129664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="40661504"/>
+        <c:axId val="109129664"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -956,7 +965,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40660928"/>
+        <c:crossAx val="109129088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1213,11 +1222,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="40663808"/>
-        <c:axId val="40664384"/>
+        <c:axId val="109131968"/>
+        <c:axId val="109132544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="40663808"/>
+        <c:axId val="109131968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1246,12 +1255,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40664384"/>
+        <c:crossAx val="109132544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="40664384"/>
+        <c:axId val="109132544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1280,7 +1289,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40663808"/>
+        <c:crossAx val="109131968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1556,11 +1565,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="95684288"/>
-        <c:axId val="95684864"/>
+        <c:axId val="129500288"/>
+        <c:axId val="129500864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95684288"/>
+        <c:axId val="129500288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1589,12 +1598,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95684864"/>
+        <c:crossAx val="129500864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95684864"/>
+        <c:axId val="129500864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1624,7 +1633,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95684288"/>
+        <c:crossAx val="129500288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1743,11 +1752,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="40938304"/>
-        <c:axId val="40937728"/>
+        <c:axId val="129503168"/>
+        <c:axId val="129503744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="40938304"/>
+        <c:axId val="129503168"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1778,12 +1787,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40937728"/>
+        <c:crossAx val="129503744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="40937728"/>
+        <c:axId val="129503744"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1814,7 +1823,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40938304"/>
+        <c:crossAx val="129503168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1928,11 +1937,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="40959296"/>
-        <c:axId val="40958720"/>
+        <c:axId val="129505472"/>
+        <c:axId val="129506048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="40959296"/>
+        <c:axId val="129505472"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1968,12 +1977,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40958720"/>
+        <c:crossAx val="129506048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="40958720"/>
+        <c:axId val="129506048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2003,7 +2012,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40959296"/>
+        <c:crossAx val="129505472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2503,8 +2512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M138"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="U71" sqref="U71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2749,7 +2758,7 @@
         <v>8.6363999999999996E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>2.8393999999999999</v>
       </c>
@@ -2766,12 +2775,12 @@
         <v>0.19592000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -2785,13 +2794,16 @@
         <v>8</v>
       </c>
       <c r="E27">
+        <v>12</v>
+      </c>
+      <c r="F27">
         <v>16</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -2804,14 +2816,14 @@
       <c r="D28">
         <v>5.7969999999999997</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>5.5789999999999997</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>6.3559999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -2824,14 +2836,14 @@
       <c r="D29">
         <v>77.325000000000003</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>51.884999999999998</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>44.828000000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -2844,10 +2856,10 @@
       <c r="D30">
         <v>390.072</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>234.83599999999998</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>195.92000000000002</v>
       </c>
     </row>
@@ -3721,7 +3733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>

</xml_diff>